<commit_message>
regression results table computed
</commit_message>
<xml_diff>
--- a/regression-results/Regression-table.xlsx
+++ b/regression-results/Regression-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sifaat\FFC-Forecasting-Study\forecasting-study\regression-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1C5E9B-336F-4146-9A12-C5FF5B53D86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674DF835-420E-4099-AA93-352E0449B4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,10 +122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -163,19 +163,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326130C5-0562-48AA-9514-354D19C603CB}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +469,7 @@
     <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -498,297 +495,261 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>-2915.44</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>-1.3541849999999999E-2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>16.25111003</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>103.3694936</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>75.396635810000006</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="6">
         <v>-9.1130000000000003E-5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>5.3950910600000004</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>2217.4258603600001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4.9074799999999997E-3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>13.68300412</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>92.064107320000005</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>20.2250774</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>3.5723999999999999E-4</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>2.7128074099999999</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>-1.3149999999999999</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>-2.7589999999999999</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>1.1879999999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>1.123</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>3.7280000000000002</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>-0.255</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>1.9890000000000001</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.20211999999999999</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1.1440000000000001E-2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.24762000000000001</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.27362999999999998</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>1.17E-3</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>0.80101999999999995</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>5.9310000000000002E-2</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="7">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5">
         <v>25260.869569999999</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <v>133.78</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>23.01</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="5">
         <v>16.648929800000001</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>211561</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="5">
         <v>45.750175400000003</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="8">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5">
         <v>28627.372567070001</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="5">
         <v>4.3487205800000002</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="5">
         <v>0.67129057000000003</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="5">
         <v>7.8548224500000003</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <v>441331.52875244</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="5">
         <v>65.450477980000002</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
         <v>0.89949999999999997</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
         <v>0.87209999999999999</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -799,7 +760,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CA9C74-857E-44B5-B866-D08E3AF468BA}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
@@ -810,7 +771,7 @@
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -833,159 +794,60 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1042,71 +904,26 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1115,114 +932,76 @@
       <c r="C7">
         <v>25260.869569999999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>133.78</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>23.01</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>16.648929800000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>211561</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
         <v>45.750175400000003</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>0.37596190000000002</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>0.97050139999999996</v>
       </c>
-      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>28627.372567070001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>4.3487205800000002</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>0.67129057000000003</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>7.8548224500000003</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>441331.52875244</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
         <v>65.450477980000002</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>8.0331959999999994E-2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>0.15834402</v>
       </c>
-      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1275,155 +1054,56 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>